<commit_message>
Update to Speeduino 201808(2) codebase.
Basic code is identical to current Speeduino release. Previous
modifications to code have now been removed.

Additional tuner studio files included to allow access to ignition
related features only.
</commit_message>
<xml_diff>
--- a/reference/hardware/v0.3/BOMs/v0.3.6_bom.xlsx
+++ b/reference/hardware/v0.3/BOMs/v0.3.6_bom.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28702"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josh/Documents/Arduino/speeduino/reference/hardware/v0.3/BOMs/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAAE1B0C-7994-2D49-AB29-63DA6DF63A32}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Full Kit" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2 Channel'!$A$1:$P$45</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Full Kit'!$A$1:$Q$45</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -35,12 +36,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Josh Stewart</author>
   </authors>
   <commentList>
-    <comment ref="P1" authorId="0">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -64,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B29" authorId="0">
+    <comment ref="B29" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -93,12 +94,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Josh Stewart</author>
   </authors>
   <commentList>
-    <comment ref="B29" authorId="0">
+    <comment ref="B29" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -883,11 +884,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1292,6 +1293,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -2014,22 +2018,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:Q48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="I1" sqref="A1:I38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="18.83203125" style="19" customWidth="1"/>
     <col min="2" max="2" width="46.6640625" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="53.1640625" customWidth="1"/>
+    <col min="8" max="8" width="0" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="17.1640625" customWidth="1"/>
     <col min="10" max="11" width="28" customWidth="1"/>
     <col min="14" max="14" width="47.83203125" customWidth="1"/>
@@ -2038,7 +2043,7 @@
     <col min="17" max="17" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="27" thickBot="1">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -2091,7 +2096,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="17" thickBot="1">
       <c r="A2" s="18"/>
       <c r="B2" s="4"/>
       <c r="C2" s="3"/>
@@ -2115,7 +2120,7 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="17" thickBot="1">
       <c r="A3" s="20">
         <f t="shared" ref="A3:A10" si="1">LEN(B3)-LEN(SUBSTITUTE(B3,",",""))+1</f>
         <v>1</v>
@@ -2170,7 +2175,7 @@
         <v>Capacitor - 1x 10uF</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="17" thickBot="1">
       <c r="A4" s="20">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -2224,7 +2229,7 @@
         <v>Capacitor - 6x 0.22uF</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="17" thickBot="1">
       <c r="A5" s="20">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -2278,7 +2283,7 @@
         <v>Capacitor - 7x 0.1uF / 100nF</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="27" thickBot="1">
       <c r="A6" s="20">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -2332,7 +2337,7 @@
         <v>Capacitor - 1x 47uF</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="27" thickBot="1">
       <c r="A7" s="20">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -2387,7 +2392,7 @@
         <v>Capacitor - 1x 0.33uF</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="17" thickBot="1">
       <c r="A8" s="20">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -2442,7 +2447,7 @@
         <v>Capacitor - 2x 0.01uF</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="17" thickBot="1">
       <c r="A9" s="20">
         <f t="shared" si="1"/>
         <v>3</v>
@@ -2497,7 +2502,7 @@
         <v>Capacitor - 3x 1uF</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="17" thickBot="1">
       <c r="A10" s="20">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -2552,7 +2557,7 @@
         <v>Capacitor - 1x 4.7nF</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="17" thickBot="1">
       <c r="A11" s="18"/>
       <c r="B11" s="4"/>
       <c r="C11" s="3"/>
@@ -2576,7 +2581,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="40" thickBot="1">
       <c r="A12" s="20">
         <f>LEN(B12)-LEN(SUBSTITUTE(B12,",",""))+1</f>
         <v>1</v>
@@ -2631,7 +2636,7 @@
         <v>Diode - 1x 1N5919BG Zener</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="40" thickBot="1">
       <c r="A13" s="20">
         <f>LEN(B13)-LEN(SUBSTITUTE(B13,",",""))+1</f>
         <v>4</v>
@@ -2685,7 +2690,7 @@
         <v>Diode - 4x 1A Schottky</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="17" thickBot="1">
       <c r="A14" s="20">
         <f>LEN(B14)-LEN(SUBSTITUTE(B14,",",""))+1</f>
         <v>8</v>
@@ -2737,7 +2742,7 @@
         <v>Diode - 8x LED-Red</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="40" thickBot="1">
       <c r="A15" s="20">
         <f>LEN(B15)-LEN(SUBSTITUTE(B15,",",""))+1</f>
         <v>4</v>
@@ -2792,7 +2797,7 @@
         <v>Diode - 4x 1N4004</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="17" thickBot="1">
       <c r="A16" s="18"/>
       <c r="B16" s="4"/>
       <c r="C16" s="3"/>
@@ -2820,7 +2825,7 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" ht="27" thickBot="1">
       <c r="A17" s="20">
         <v>1</v>
       </c>
@@ -2874,7 +2879,7 @@
         <v>1x Surge Protection</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" ht="17" thickBot="1">
       <c r="A18" s="18"/>
       <c r="B18" s="4"/>
       <c r="C18" s="3"/>
@@ -2902,7 +2907,7 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" ht="40" thickBot="1">
       <c r="A19" s="20">
         <v>14</v>
       </c>
@@ -2955,7 +2960,7 @@
         <v>14x Dual Terminal Block</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" ht="17" thickBot="1">
       <c r="A20" s="20">
         <v>5</v>
       </c>
@@ -3004,7 +3009,7 @@
         <v>5x Jumper</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" ht="40" thickBot="1">
       <c r="A21" s="20">
         <v>5</v>
       </c>
@@ -3055,7 +3060,7 @@
         <v>5x 40 POS 0.100 Pin Header</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" ht="17" thickBot="1">
       <c r="A22" s="18"/>
       <c r="B22" s="4"/>
       <c r="C22" s="3"/>
@@ -3083,7 +3088,7 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" ht="27" thickBot="1">
       <c r="A23" s="20">
         <f>LEN(B23)-LEN(SUBSTITUTE(B23,",",""))+1</f>
         <v>8</v>
@@ -3139,7 +3144,7 @@
         <v>8x 62A MOSFET N-CH</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" ht="17" thickBot="1">
       <c r="A24" s="18"/>
       <c r="B24" s="4"/>
       <c r="C24" s="3"/>
@@ -3163,7 +3168,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" ht="17" thickBot="1">
       <c r="A25" s="20">
         <f>LEN(B25)-LEN(SUBSTITUTE(B25,",",""))+1</f>
         <v>1</v>
@@ -3215,7 +3220,7 @@
         <v>Resistor - 1x 10k</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" ht="27" thickBot="1">
       <c r="A26" s="20">
         <f>LEN(B26)-LEN(SUBSTITUTE(B26,",",""))+1</f>
         <v>15</v>
@@ -3267,7 +3272,7 @@
         <v>Resistor - 15x 1k</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" ht="27" thickBot="1">
       <c r="A27" s="20">
         <f>LEN(B27)-LEN(SUBSTITUTE(B27,",",""))+1</f>
         <v>4</v>
@@ -3321,7 +3326,7 @@
         <v>Resistor - 4x 680</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" ht="40" thickBot="1">
       <c r="A28" s="20">
         <f>LEN(B28)-LEN(SUBSTITUTE(B28,",",""))+1</f>
         <v>6</v>
@@ -3374,7 +3379,7 @@
         <v>Resistor - 6x 470</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" ht="17" thickBot="1">
       <c r="A29" s="20">
         <f>LEN(B29)-LEN(SUBSTITUTE(B29,",",""))+1</f>
         <v>7</v>
@@ -3425,7 +3430,7 @@
         <v>Resistor - 7x 0.1% 2.49k</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" ht="17" thickBot="1">
       <c r="A30" s="20">
         <v>1</v>
       </c>
@@ -3479,7 +3484,7 @@
         <v>Resistor - 1x 0.1% 3.9k</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" ht="17" thickBot="1">
       <c r="A31" s="20">
         <f>LEN(B31)-LEN(SUBSTITUTE(B31,",",""))+1</f>
         <v>12</v>
@@ -3531,7 +3536,7 @@
         <v>Resistor - 12x 100k</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" ht="17" thickBot="1">
       <c r="A32" s="20">
         <f>LEN(B32)-LEN(SUBSTITUTE(B32,",",""))+1</f>
         <v>4</v>
@@ -3584,7 +3589,7 @@
         <v>Resistor - 4x 160</v>
       </c>
     </row>
-    <row r="33" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" ht="17" thickBot="1">
       <c r="A33" s="18"/>
       <c r="B33" s="4"/>
       <c r="C33" s="3"/>
@@ -3608,7 +3613,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" ht="27" thickBot="1">
       <c r="A34" s="20">
         <v>1</v>
       </c>
@@ -3662,7 +3667,7 @@
         <v>1x LM2940T-5.0/NOPB</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" ht="40" thickBot="1">
       <c r="A35" s="20">
         <v>1</v>
       </c>
@@ -3715,7 +3720,7 @@
         <v>1x 1-Bar MAP sensor</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" ht="27" thickBot="1">
       <c r="A36" s="20">
         <v>2</v>
       </c>
@@ -3769,7 +3774,7 @@
         <v>2x TC4424EPA</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" ht="17" thickBot="1">
       <c r="A37" s="20">
         <v>1</v>
       </c>
@@ -3823,7 +3828,7 @@
         <v>1x SP721APP</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" ht="17" thickBot="1">
       <c r="A38" s="20">
         <v>3</v>
       </c>
@@ -3871,7 +3876,7 @@
         <v>3x IC Socket</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" ht="17" thickBot="1">
       <c r="A39" s="18"/>
       <c r="B39" s="4"/>
       <c r="C39" s="3"/>
@@ -3895,7 +3900,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" ht="17" thickBot="1">
       <c r="A40" s="18">
         <v>0</v>
       </c>
@@ -3926,7 +3931,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" ht="17" thickBot="1">
       <c r="A41" s="18"/>
       <c r="B41" s="4"/>
       <c r="C41" s="3"/>
@@ -3950,7 +3955,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" ht="17" thickBot="1">
       <c r="A42" s="18"/>
       <c r="B42" s="4" t="s">
         <v>75</v>
@@ -3976,7 +3981,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" ht="17" thickBot="1">
       <c r="A43" s="18">
         <v>1</v>
       </c>
@@ -4015,7 +4020,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" ht="17" thickBot="1">
       <c r="A44" s="18">
         <v>1</v>
       </c>
@@ -4045,7 +4050,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" ht="17" thickBot="1">
       <c r="A45" s="18"/>
       <c r="B45" s="4"/>
       <c r="C45" s="3"/>
@@ -4074,52 +4079,52 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17">
       <c r="P46" t="str">
         <f t="shared" ref="P46" si="15">IF(NOT(E46=""),E46&amp;"|"&amp;#REF!,"")</f>
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:17">
       <c r="P47" t="str">
         <f t="shared" ref="P47" si="16">IF(NOT(E47=""),E47&amp;"|"&amp;#REF!,"")</f>
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:17">
       <c r="P48" t="str">
         <f t="shared" ref="P48" si="17">IF(NOT(E48=""),E48&amp;"|"&amp;#REF!,"")</f>
         <v/>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q45"/>
+  <autoFilter ref="A1:Q45" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="1">
     <mergeCell ref="I45:J45"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="J6" r:id="rId1" display="478-1910-ND"/>
-    <hyperlink ref="J13" r:id="rId2" display="1N5818-TPCT-ND"/>
-    <hyperlink ref="J17" r:id="rId3"/>
-    <hyperlink ref="J25" r:id="rId4" display="10.0KXBK-ND"/>
-    <hyperlink ref="J30" r:id="rId5"/>
-    <hyperlink ref="J31" r:id="rId6"/>
-    <hyperlink ref="J35" r:id="rId7"/>
-    <hyperlink ref="J3" r:id="rId8" display="478-1842-ND"/>
-    <hyperlink ref="J7" r:id="rId9" display="445-5312-ND"/>
-    <hyperlink ref="J8" r:id="rId10" display="399-4148-ND"/>
-    <hyperlink ref="J29" r:id="rId11" display="985-1047-1-ND"/>
+    <hyperlink ref="J6" r:id="rId1" display="478-1910-ND" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="J13" r:id="rId2" display="1N5818-TPCT-ND" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="J17" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="J25" r:id="rId4" display="10.0KXBK-ND" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="J30" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="J31" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="J35" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="J3" r:id="rId8" display="478-1842-ND" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="J7" r:id="rId9" display="445-5312-ND" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="J8" r:id="rId10" display="399-4148-ND" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="J29" r:id="rId11" display="985-1047-1-ND" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="58" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" scale="33" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" copies="2"/>
   <legacyDrawing r:id="rId12"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:P45"/>
@@ -4128,7 +4133,7 @@
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="18.83203125" style="19" customWidth="1"/>
     <col min="2" max="2" width="46.6640625" customWidth="1"/>
@@ -4143,7 +4148,7 @@
     <col min="16" max="16" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="27" thickBot="1">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -4193,7 +4198,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="17" thickBot="1">
       <c r="A2" s="18"/>
       <c r="B2" s="4"/>
       <c r="C2" s="3"/>
@@ -4217,7 +4222,7 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="17" thickBot="1">
       <c r="A3" s="20">
         <f t="shared" ref="A3:A10" si="0">LEN(B3)-LEN(SUBSTITUTE(B3,",",""))+1</f>
         <v>1</v>
@@ -4267,7 +4272,7 @@
         <v>Capacitor - 1x 10uF</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="17" thickBot="1">
       <c r="A4" s="20">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -4317,7 +4322,7 @@
         <v>Capacitor - 6x 0.22uF</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="27" thickBot="1">
       <c r="A5" s="20">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -4367,7 +4372,7 @@
         <v>Capacitor - 7x 0.1uF / 100nF</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="17" thickBot="1">
       <c r="A6" s="20">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4417,7 +4422,7 @@
         <v>Capacitor - 1x 47uF</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="17" thickBot="1">
       <c r="A7" s="20">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4467,7 +4472,7 @@
         <v>Capacitor - 1x 0.33uF</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="17" thickBot="1">
       <c r="A8" s="20">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -4517,7 +4522,7 @@
         <v>Capacitor - 2x 0.01uF</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="17" thickBot="1">
       <c r="A9" s="20">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -4567,7 +4572,7 @@
         <v>Capacitor - 2x 1uF</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="17" thickBot="1">
       <c r="A10" s="20">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4615,7 +4620,7 @@
         <v>Capacitor - 1x 4.7nF</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="17" thickBot="1">
       <c r="A11" s="18"/>
       <c r="B11" s="4"/>
       <c r="C11" s="3"/>
@@ -4635,7 +4640,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="27" thickBot="1">
       <c r="A12" s="20">
         <f>LEN(B12)-LEN(SUBSTITUTE(B12,",",""))+1</f>
         <v>1</v>
@@ -4685,7 +4690,7 @@
         <v>Diode - 1x 1N5919BG Zener</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="27" thickBot="1">
       <c r="A13" s="20">
         <f>LEN(B13)-LEN(SUBSTITUTE(B13,",",""))+1</f>
         <v>4</v>
@@ -4735,7 +4740,7 @@
         <v>Diode - 4x 1N5818-TP Schottky</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="17" thickBot="1">
       <c r="A14" s="20">
         <f>LEN(B14)-LEN(SUBSTITUTE(B14,",",""))+1</f>
         <v>4</v>
@@ -4779,7 +4784,7 @@
         <v>Diode - 4x LED-Red</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="27" thickBot="1">
       <c r="A15" s="20">
         <f>LEN(B15)-LEN(SUBSTITUTE(B15,",",""))+1</f>
         <v>2</v>
@@ -4829,7 +4834,7 @@
         <v>Diode - 2x 1N4004</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="17" thickBot="1">
       <c r="A16" s="18"/>
       <c r="B16" s="4"/>
       <c r="C16" s="3"/>
@@ -4853,7 +4858,7 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="17" thickBot="1">
       <c r="A17" s="20">
         <v>1</v>
       </c>
@@ -4902,7 +4907,7 @@
         <v>1x Surge Protection</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="17" thickBot="1">
       <c r="A18" s="18"/>
       <c r="B18" s="4"/>
       <c r="C18" s="3"/>
@@ -4926,7 +4931,7 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" ht="27" thickBot="1">
       <c r="A19" s="20">
         <v>14</v>
       </c>
@@ -4973,7 +4978,7 @@
         <v>14x Dual Terminal Block</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" ht="17" thickBot="1">
       <c r="A20" s="20">
         <v>5</v>
       </c>
@@ -5014,7 +5019,7 @@
         <v>5x Jumper</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" ht="27" thickBot="1">
       <c r="A21" s="20">
         <v>5</v>
       </c>
@@ -5061,7 +5066,7 @@
         <v>5x 40 POS 0.100 Pin Header</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" ht="17" thickBot="1">
       <c r="A22" s="18"/>
       <c r="B22" s="4"/>
       <c r="C22" s="3"/>
@@ -5085,7 +5090,7 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" ht="27" thickBot="1">
       <c r="A23" s="20">
         <v>6</v>
       </c>
@@ -5136,7 +5141,7 @@
         <v>6x 62A MOSFET N-CH</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" ht="17" thickBot="1">
       <c r="A24" s="18"/>
       <c r="B24" s="4"/>
       <c r="C24" s="3"/>
@@ -5156,7 +5161,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" ht="17" thickBot="1">
       <c r="A25" s="20">
         <f t="shared" ref="A25:A32" si="5">LEN(B25)-LEN(SUBSTITUTE(B25,",",""))+1</f>
         <v>3</v>
@@ -5204,7 +5209,7 @@
         <v>Resistor - 3x 10k</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" ht="17" thickBot="1">
       <c r="A26" s="20">
         <f t="shared" si="5"/>
         <v>9</v>
@@ -5252,7 +5257,7 @@
         <v>Resistor - 9x 1k</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" ht="31" customHeight="1" thickBot="1">
       <c r="A27" s="20">
         <f t="shared" si="5"/>
         <v>4</v>
@@ -5298,7 +5303,7 @@
         <v>Resistor - 4x 680</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" ht="27" thickBot="1">
       <c r="A28" s="20">
         <f t="shared" si="5"/>
         <v>6</v>
@@ -5346,7 +5351,7 @@
         <v>Resistor - 6x 470</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="27" thickBot="1">
       <c r="A29" s="20">
         <f t="shared" si="5"/>
         <v>3</v>
@@ -5395,7 +5400,7 @@
         <v>Resistor - 3x 0.1% 2.49k</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" ht="17" thickBot="1">
       <c r="A30" s="20">
         <f t="shared" si="5"/>
         <v>1</v>
@@ -5445,7 +5450,7 @@
         <v>Resistor - 1x 0.1% 3.9k</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" ht="17" thickBot="1">
       <c r="A31" s="20">
         <f t="shared" si="5"/>
         <v>8</v>
@@ -5493,7 +5498,7 @@
         <v>Resistor - 8x 100k</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" ht="17" thickBot="1">
       <c r="A32" s="20">
         <f t="shared" si="5"/>
         <v>2</v>
@@ -5541,7 +5546,7 @@
         <v>Resistor - 2x 160</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" ht="17" thickBot="1">
       <c r="A33" s="18"/>
       <c r="B33" s="4"/>
       <c r="C33" s="3"/>
@@ -5561,7 +5566,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" ht="27" thickBot="1">
       <c r="A34" s="20">
         <v>1</v>
       </c>
@@ -5610,7 +5615,7 @@
         <v>1x LM2940T-5.0/NOPB</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" ht="27" thickBot="1">
       <c r="A35" s="20">
         <v>1</v>
       </c>
@@ -5655,7 +5660,7 @@
         <v>1x 1-Bar MAP sensor</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" ht="27" thickBot="1">
       <c r="A36" s="20">
         <v>1</v>
       </c>
@@ -5702,7 +5707,7 @@
         <v>1x TC4424EPA</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" ht="17" thickBot="1">
       <c r="A37" s="20">
         <v>1</v>
       </c>
@@ -5749,7 +5754,7 @@
         <v>1x SP721APP</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" ht="17" thickBot="1">
       <c r="A38" s="20">
         <v>3</v>
       </c>
@@ -5790,7 +5795,7 @@
         <v>3x IC Socket</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" ht="17" thickBot="1">
       <c r="A39" s="18"/>
       <c r="B39" s="4"/>
       <c r="C39" s="3"/>
@@ -5810,7 +5815,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" ht="17" thickBot="1">
       <c r="A40" s="18">
         <v>0</v>
       </c>
@@ -5839,7 +5844,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" ht="17" thickBot="1">
       <c r="A41" s="18"/>
       <c r="B41" s="4"/>
       <c r="C41" s="3"/>
@@ -5859,7 +5864,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" ht="17" thickBot="1">
       <c r="A42" s="18"/>
       <c r="B42" s="4" t="s">
         <v>75</v>
@@ -5881,7 +5886,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" ht="17" thickBot="1">
       <c r="A43" s="18">
         <v>1</v>
       </c>
@@ -5918,7 +5923,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" ht="17" thickBot="1">
       <c r="A44" s="18">
         <v>1</v>
       </c>
@@ -5944,7 +5949,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" ht="17" thickBot="1">
       <c r="A45" s="18"/>
       <c r="B45" s="4"/>
       <c r="C45" s="3"/>
@@ -5970,23 +5975,23 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P45"/>
+  <autoFilter ref="A1:P45" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <mergeCells count="1">
     <mergeCell ref="J45:K45"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="K3" r:id="rId1" display="478-1842-ND"/>
-    <hyperlink ref="K7" r:id="rId2" display="445-5312-ND"/>
-    <hyperlink ref="K8" r:id="rId3" display="399-4148-ND"/>
-    <hyperlink ref="K13" r:id="rId4"/>
-    <hyperlink ref="K17" r:id="rId5"/>
-    <hyperlink ref="K25" r:id="rId6" display="10.0KXBK-ND"/>
-    <hyperlink ref="K30" r:id="rId7"/>
-    <hyperlink ref="K31" r:id="rId8"/>
-    <hyperlink ref="K35" r:id="rId9"/>
-    <hyperlink ref="K6" r:id="rId10" display="478-1910-ND"/>
-    <hyperlink ref="J29" r:id="rId11" display="985-1047-1-ND"/>
+    <hyperlink ref="K3" r:id="rId1" display="478-1842-ND" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="K7" r:id="rId2" display="445-5312-ND" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="K8" r:id="rId3" display="399-4148-ND" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="K13" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="K17" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="K25" r:id="rId6" display="10.0KXBK-ND" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="K30" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="K31" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="K35" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="K6" r:id="rId10" display="478-1910-ND" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="J29" r:id="rId11" display="985-1047-1-ND" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
   </hyperlinks>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="34" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>